<commit_message>
Added support for unnamed groups in matching pattern
Also added additional test case data.
</commit_message>
<xml_diff>
--- a/EventPatterns.xlsx
+++ b/EventPatterns.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
   <si>
     <t>Type</t>
   </si>
@@ -66,10 +66,22 @@
     <t>No production logic(.*)</t>
   </si>
   <si>
+    <t>OldLogFilesMoved</t>
+  </si>
+  <si>
+    <t>Old log files moved (into|to)\s*(?P&lt;_folder&gt;.*)</t>
+  </si>
+  <si>
     <t>XMLTransactionFailure</t>
   </si>
   <si>
     <t>Transaction Failure Exception, Fatality = 1, NotificationTitle = "HTTPXMLBackEndError", NotificationText = ""</t>
+  </si>
+  <si>
+    <t>NoBackendsLoaded</t>
+  </si>
+  <si>
+    <t>(?P&lt;user&gt;.*): No backends loaded.(?P&lt;_errorDetail&gt;.*)</t>
   </si>
   <si>
     <t>AlreadyLoggedIn</t>
@@ -284,10 +296,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -305,8 +317,87 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,7 +411,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,62 +434,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -411,39 +447,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -464,13 +476,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,13 +626,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,151 +656,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,26 +714,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -736,6 +748,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -765,21 +792,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -802,15 +814,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -820,130 +832,130 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1023,9 +1035,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1_3" displayName="Table1_3" ref="A1:G8" totalsRowShown="0">
-  <autoFilter ref="A1:G8"/>
-  <sortState ref="A1:G8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1_3" displayName="Table1_3" ref="A1:G10" totalsRowShown="0">
+  <autoFilter ref="A1:G10"/>
+  <sortState ref="A1:G10">
     <sortCondition ref="G1:G37"/>
   </sortState>
   <tableColumns count="7">
@@ -1319,13 +1331,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelRow="7" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="7.625" customWidth="1"/>
     <col min="2" max="2" width="8.625" customWidth="1"/>
@@ -1440,15 +1452,9 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="8">
-        <v>1</v>
-      </c>
-      <c r="B6" s="8">
-        <v>24</v>
-      </c>
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
         <v>16</v>
@@ -1460,13 +1466,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C7" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
@@ -1478,17 +1484,55 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="A8" s="8">
+        <v>0</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>6</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="8">
+        <v>0</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>6</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
         <v>22</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1530,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1542,7 +1586,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1556,11 +1600,11 @@
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1574,13 +1618,13 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1594,13 +1638,13 @@
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1614,11 +1658,11 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1632,10 +1676,10 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -1650,7 +1694,7 @@
         <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1664,10 +1708,10 @@
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1681,13 +1725,13 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" t="s">
         <v>40</v>
       </c>
-      <c r="G9" t="s">
-        <v>36</v>
-      </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1707,10 +1751,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1724,7 +1768,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1738,7 +1782,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1755,13 +1799,13 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1775,10 +1819,10 @@
         <v>26</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1792,7 +1836,7 @@
         <v>26</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -1807,7 +1851,7 @@
         <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1821,7 +1865,7 @@
         <v>26</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1836,10 +1880,10 @@
         <v>26</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H18" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" ht="31.2" spans="1:8">
@@ -1853,7 +1897,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -1868,10 +1912,10 @@
         <v>26</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1885,7 +1929,7 @@
         <v>26</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1899,7 +1943,7 @@
         <v>26</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H22" s="1"/>
     </row>
@@ -1914,7 +1958,7 @@
         <v>26</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1929,10 +1973,10 @@
         <v>26</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1946,7 +1990,7 @@
         <v>26</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -1961,11 +2005,11 @@
         <v>26</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1979,11 +2023,11 @@
         <v>26</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1997,7 +2041,7 @@
         <v>26</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2011,10 +2055,10 @@
         <v>26</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H29" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2028,10 +2072,10 @@
         <v>26</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H30" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2045,10 +2089,10 @@
         <v>26</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2062,7 +2106,7 @@
         <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -2077,7 +2121,7 @@
         <v>18</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G33" t="s">
         <v>13</v>
@@ -2109,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -2124,10 +2168,10 @@
         <v>22</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H36" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2141,10 +2185,10 @@
         <v>18</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2169,37 +2213,37 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support optional named groups
Also fixed issue with showing subpatterns when parent pattern had no other occurances.
Added test data
</commit_message>
<xml_diff>
--- a/EventPatterns.xlsx
+++ b/EventPatterns.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23028" windowHeight="9804"/>
+    <workbookView windowWidth="21216" windowHeight="9504"/>
   </bookViews>
   <sheets>
     <sheet name="TopPatterns" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
   <si>
     <t>Type</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>com.syclo.agentry.BusinessLogicException:(?P&lt;errorDetail&gt;.*)</t>
+  </si>
+  <si>
+    <t>ThreadInUse</t>
+  </si>
+  <si>
+    <t>com.syclo.agentry.BusinessLogicException: (|(?P&lt;steplet&gt;.*)Steplet - )\s*The context with the session id (?P&lt;sessionId&gt;.*) scope type \[null\] is currently used in thread (?P&lt;thread1&gt;.*).Current thread is (?P&lt;_thread2&gt;.*).(?P&lt;_errorDetail&gt;.*)</t>
   </si>
   <si>
     <t>Steplet</t>
@@ -314,14 +320,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -365,7 +363,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -380,16 +378,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,29 +431,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -437,6 +442,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -453,13 +466,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -500,19 +506,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -524,139 +554,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -786,8 +792,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -795,8 +801,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -814,7 +820,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -832,130 +838,130 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1035,9 +1041,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1_3" displayName="Table1_3" ref="A1:G10" totalsRowShown="0">
-  <autoFilter ref="A1:G10"/>
-  <sortState ref="A1:G10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1_3" displayName="Table1_3" ref="A1:G11" totalsRowShown="0">
+  <autoFilter ref="A1:G11"/>
+  <sortState ref="A1:G11">
     <sortCondition ref="G1:G37"/>
   </sortState>
   <tableColumns count="7">
@@ -1331,10 +1337,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="6"/>
@@ -1391,15 +1397,9 @@
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8">
-        <v>20</v>
-      </c>
-      <c r="C3" s="8">
-        <v>26</v>
-      </c>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
@@ -1419,18 +1419,18 @@
         <v>20</v>
       </c>
       <c r="C4" s="8">
-        <v>18</v>
-      </c>
-      <c r="D4" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="8">
@@ -1440,21 +1440,29 @@
         <v>20</v>
       </c>
       <c r="C5" s="8">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8">
+        <v>20</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
         <v>16</v>
@@ -1465,15 +1473,9 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="8">
-        <v>1</v>
-      </c>
-      <c r="B7" s="8">
-        <v>24</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
         <v>18</v>
@@ -1485,13 +1487,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C8" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
@@ -1522,17 +1524,36 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="A10" s="8">
+        <v>0</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>26</v>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1574,7 +1595,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1586,7 +1607,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1600,11 +1621,11 @@
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1618,13 +1639,13 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1638,13 +1659,13 @@
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1658,11 +1679,11 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1676,10 +1697,10 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -1694,7 +1715,7 @@
         <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1708,10 +1729,10 @@
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1725,13 +1746,13 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1751,10 +1772,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1768,7 +1789,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1782,7 +1803,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1799,13 +1820,13 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1819,10 +1840,10 @@
         <v>26</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1836,7 +1857,7 @@
         <v>26</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -1851,7 +1872,7 @@
         <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1865,7 +1886,7 @@
         <v>26</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1880,10 +1901,10 @@
         <v>26</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" ht="31.2" spans="1:8">
@@ -1897,7 +1918,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -1912,10 +1933,10 @@
         <v>26</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1929,7 +1950,7 @@
         <v>26</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1943,7 +1964,7 @@
         <v>26</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H22" s="1"/>
     </row>
@@ -1958,7 +1979,7 @@
         <v>26</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1973,10 +1994,10 @@
         <v>26</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1990,7 +2011,7 @@
         <v>26</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -2005,11 +2026,11 @@
         <v>26</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2023,11 +2044,11 @@
         <v>26</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2041,7 +2062,7 @@
         <v>26</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2055,10 +2076,10 @@
         <v>26</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2072,10 +2093,10 @@
         <v>26</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2089,10 +2110,10 @@
         <v>26</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2106,7 +2127,7 @@
         <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -2121,10 +2142,10 @@
         <v>18</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G33" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H33" s="1"/>
     </row>
@@ -2139,7 +2160,7 @@
         <v>3</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2153,7 +2174,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -2168,10 +2189,10 @@
         <v>22</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2185,10 +2206,10 @@
         <v>18</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2213,37 +2234,37 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIxed Issue with skipping detailed group
Prior to fix, values in skipped group would show as the values in the next group.
</commit_message>
<xml_diff>
--- a/EventPatterns.xlsx
+++ b/EventPatterns.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
   <si>
     <t>Type</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>com.syclo.agentry.BusinessLogicException: (|(?P&lt;steplet&gt;.*)Steplet - )\s*The context with the session id (?P&lt;sessionId&gt;.*) scope type \[null\] is currently used in thread (?P&lt;thread1&gt;.*).Current thread is (?P&lt;_thread2&gt;.*).(?P&lt;_errorDetail&gt;.*)</t>
+  </si>
+  <si>
+    <t>CX_SY_NO_HANDLER</t>
+  </si>
+  <si>
+    <t>com.syclo.agentry.BusinessLogicException: (?P&lt;steplet&gt;.*)Steplet - (|(?P&lt;_time&gt;.*) - )CX_SY_NO_HANDLER: An exception of type '(?P&lt;exceptionType&gt;.*)' occured, that was not caught anywhere in the call hierarchy. It was not handled locally or declared using a raising cl</t>
   </si>
   <si>
     <t>Steplet</t>
@@ -302,10 +308,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -323,32 +329,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,9 +345,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -378,45 +382,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -431,15 +407,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -453,10 +421,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -466,6 +443,35 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -482,19 +488,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,7 +584,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,151 +668,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,24 +728,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -760,16 +762,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -798,29 +809,24 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -838,130 +844,130 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1041,9 +1047,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1_3" displayName="Table1_3" ref="A1:G11" totalsRowShown="0">
-  <autoFilter ref="A1:G11"/>
-  <sortState ref="A1:G11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1_3" displayName="Table1_3" ref="A1:G12" totalsRowShown="0">
+  <autoFilter ref="A1:G12"/>
+  <sortState ref="A1:G12">
     <sortCondition ref="G1:G37"/>
   </sortState>
   <tableColumns count="7">
@@ -1337,7 +1343,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -1412,15 +1418,9 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="8">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8">
-        <v>20</v>
-      </c>
-      <c r="C4" s="8">
-        <v>26</v>
-      </c>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="8" t="s">
         <v>7</v>
       </c>
@@ -1440,18 +1440,18 @@
         <v>20</v>
       </c>
       <c r="C5" s="8">
-        <v>18</v>
-      </c>
-      <c r="D5" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="E5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="8">
@@ -1461,21 +1461,29 @@
         <v>20</v>
       </c>
       <c r="C6" s="8">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
         <v>18</v>
@@ -1486,15 +1494,9 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="8">
-        <v>24</v>
-      </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
         <v>20</v>
@@ -1506,13 +1508,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C9" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
@@ -1543,17 +1545,36 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="A11" s="8">
+        <v>0</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>6</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>28</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1595,7 +1616,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1607,7 +1628,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1621,11 +1642,11 @@
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1639,13 +1660,13 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1659,13 +1680,13 @@
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1679,11 +1700,11 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1697,10 +1718,10 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -1715,7 +1736,7 @@
         <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1729,10 +1750,10 @@
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1746,13 +1767,13 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1772,10 +1793,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1789,7 +1810,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1803,7 +1824,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1820,13 +1841,13 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1840,10 +1861,10 @@
         <v>26</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1857,7 +1878,7 @@
         <v>26</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -1872,7 +1893,7 @@
         <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1886,7 +1907,7 @@
         <v>26</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1901,10 +1922,10 @@
         <v>26</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" ht="31.2" spans="1:8">
@@ -1918,7 +1939,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -1933,10 +1954,10 @@
         <v>26</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1950,7 +1971,7 @@
         <v>26</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1964,7 +1985,7 @@
         <v>26</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H22" s="1"/>
     </row>
@@ -1979,7 +2000,7 @@
         <v>26</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1994,10 +2015,10 @@
         <v>26</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2011,7 +2032,7 @@
         <v>26</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -2026,11 +2047,11 @@
         <v>26</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2044,11 +2065,11 @@
         <v>26</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2062,7 +2083,7 @@
         <v>26</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2076,10 +2097,10 @@
         <v>26</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2093,10 +2114,10 @@
         <v>26</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2110,10 +2131,10 @@
         <v>26</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2127,7 +2148,7 @@
         <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -2142,10 +2163,10 @@
         <v>18</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H33" s="1"/>
     </row>
@@ -2160,7 +2181,7 @@
         <v>3</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2174,7 +2195,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -2189,10 +2210,10 @@
         <v>22</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2206,10 +2227,10 @@
         <v>18</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2234,37 +2255,37 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>